<commit_message>
curlsmith E2E testcase & testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74215308-35B0-4CE8-B02F-BD192F73DC13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468A6A1B-827C-4858-B274-7C5763990BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>UserName</t>
   </si>
@@ -143,19 +143,84 @@
   </si>
   <si>
     <t>scent</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>AccountDetails</t>
+  </si>
+  <si>
+    <t>Curl Defining Styling Soufflé (Mini 2 fl oz.)</t>
+  </si>
+  <si>
+    <t>vnarra@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>avayugundla@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Lotuswave@123</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Qa</t>
+  </si>
+  <si>
+    <t>Configurable Product</t>
+  </si>
+  <si>
+    <t>Mini 2 fl oz.</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>844 N Colony Rd</t>
+  </si>
+  <si>
+    <t>Wallingford</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>06492</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -181,14 +246,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO1"/>
+  <dimension ref="A1:AO5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,8 +697,101 @@
         <v>37</v>
       </c>
     </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="X4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" t="s">
+        <v>54</v>
+      </c>
+      <c r="P5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>56</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="S5">
+        <v>9898989898</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{CC7365F0-057F-4E26-AB1D-C83143B00E3B}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{6EC0626A-93FF-4B75-9E55-AED6062E6D4B}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{F0A4EEF5-EEBE-4FF0-BB4D-64D8943AC215}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
+    <hyperlink ref="K5" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
6 testcase for curlsmith
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AEB4DA-BE8E-4EEB-974E-5147CB3D06D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206839CB-7A6A-4862-B29C-3F8378142341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>UserName</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>curl-transition-kit</t>
+  </si>
+  <si>
+    <t>Simple_product_10qty</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Configurable Product_10qty</t>
   </si>
 </sst>
 </file>
@@ -581,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL10"/>
+  <dimension ref="A1:AL12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
@@ -733,7 +742,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>42</v>
@@ -800,24 +809,24 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="20.25">
+    <row r="5" spans="1:38">
       <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="U5" t="s">
+        <v>40</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y5" s="4"/>
+    </row>
+    <row r="6" spans="1:38" ht="20.25">
+      <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="U5" s="7" t="s">
+      <c r="U6" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y5" s="4"/>
-    </row>
-    <row r="6" spans="1:38">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="U6" t="s">
-        <v>60</v>
       </c>
       <c r="V6" s="5" t="s">
         <v>48</v>
@@ -826,87 +835,111 @@
     </row>
     <row r="7" spans="1:38">
       <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L7" t="s">
-        <v>50</v>
-      </c>
-      <c r="M7" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7" t="s">
-        <v>52</v>
-      </c>
-      <c r="O7" t="s">
-        <v>53</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q7">
-        <v>9898989898</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="U7" t="s">
+        <v>60</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y7" s="4"/>
     </row>
     <row r="8" spans="1:38">
       <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="R8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>57</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="U8" t="s">
+        <v>60</v>
+      </c>
+      <c r="V8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y8" s="4"/>
     </row>
     <row r="9" spans="1:38">
       <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" t="s">
+        <v>52</v>
+      </c>
+      <c r="O9" t="s">
+        <v>53</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9">
+        <v>9898989898</v>
       </c>
     </row>
     <row r="10" spans="1:38">
       <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38">
+      <c r="A12" t="s">
         <v>61</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F12" t="s">
         <v>44</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G12" t="s">
         <v>66</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L12" t="s">
         <v>62</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M12" t="s">
         <v>64</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N12" t="s">
         <v>52</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="P10" s="5" t="s">
+      <c r="P12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Q10">
+      <c r="Q12">
         <v>9999999999</v>
       </c>
     </row>
@@ -916,9 +949,9 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6EC0626A-93FF-4B75-9E55-AED6062E6D4B}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{F0A4EEF5-EEBE-4FF0-BB4D-64D8943AC215}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
-    <hyperlink ref="K7" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
+    <hyperlink ref="K9" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
+    <hyperlink ref="D11" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
7th testcase for the E2E curlsmith
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{206839CB-7A6A-4862-B29C-3F8378142341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAF3641-A5AE-4A86-BB13-4F8C9F4989CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1965" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="73">
   <si>
     <t>UserName</t>
   </si>
@@ -208,18 +208,6 @@
     <t>Different_Bill_Ship</t>
   </si>
   <si>
-    <t>2 Dream Valley Drive</t>
-  </si>
-  <si>
-    <t>19073</t>
-  </si>
-  <si>
-    <t>Newtown Square</t>
-  </si>
-  <si>
-    <t>Pennsylvania</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
@@ -236,6 +224,21 @@
   </si>
   <si>
     <t>Configurable Product_10qty</t>
+  </si>
+  <si>
+    <t>No Tax Address</t>
+  </si>
+  <si>
+    <t>844 North Court</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>12211</t>
   </si>
 </sst>
 </file>
@@ -590,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL12"/>
+  <dimension ref="A1:AL13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
@@ -760,19 +763,19 @@
         <v>45</v>
       </c>
       <c r="L2" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="M2" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="N2" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>65</v>
+      <c r="O2" t="s">
+        <v>71</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="Q2">
         <v>9999999999</v>
@@ -780,21 +783,40 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" t="s">
-        <v>40</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
+        <v>68</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3">
+        <v>9898989898</v>
       </c>
     </row>
     <row r="4" spans="1:38">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="U4" t="s">
         <v>40</v>
@@ -805,40 +827,42 @@
       <c r="X4">
         <v>1</v>
       </c>
-      <c r="Y4" s="4" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="5" spans="1:38">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="U5" t="s">
         <v>40</v>
       </c>
       <c r="V5" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="Y5" s="4"/>
-    </row>
-    <row r="6" spans="1:38" ht="20.25">
+        <v>48</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38">
       <c r="A6" t="s">
         <v>67</v>
       </c>
-      <c r="U6" s="7" t="s">
-        <v>68</v>
+      <c r="U6" t="s">
+        <v>40</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" ht="20.25">
       <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="U7" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="U7" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="V7" s="5" t="s">
         <v>48</v>
@@ -847,99 +871,111 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="U8" t="s">
         <v>60</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="Y8" s="4"/>
     </row>
     <row r="9" spans="1:38">
       <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
-      </c>
-      <c r="M9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" t="s">
-        <v>52</v>
-      </c>
-      <c r="O9" t="s">
-        <v>53</v>
-      </c>
-      <c r="P9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q9">
-        <v>9898989898</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="U9" t="s">
+        <v>60</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y9" s="4"/>
     </row>
     <row r="10" spans="1:38">
       <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="R10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" t="s">
+        <v>52</v>
+      </c>
+      <c r="O10" t="s">
+        <v>71</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q10">
+        <v>9898989898</v>
       </c>
     </row>
     <row r="11" spans="1:38">
       <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:38">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38">
+      <c r="A13" t="s">
         <v>61</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>44</v>
       </c>
-      <c r="G12" t="s">
-        <v>66</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="G13" t="s">
         <v>62</v>
       </c>
-      <c r="M12" t="s">
-        <v>64</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="L13" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N13" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q12">
+      <c r="O13" t="s">
+        <v>71</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q13">
         <v>9999999999</v>
       </c>
     </row>
@@ -949,9 +985,9 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6EC0626A-93FF-4B75-9E55-AED6062E6D4B}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{F0A4EEF5-EEBE-4FF0-BB4D-64D8943AC215}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
-    <hyperlink ref="K9" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
-    <hyperlink ref="B11" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
-    <hyperlink ref="D11" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
+    <hyperlink ref="K10" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
+    <hyperlink ref="B12" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
2 testcase changes for the curlsmith
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C20133-C63A-44D3-AADC-FBC19B156454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1370A751-8062-4B22-A03D-B28DADC40F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,9 +187,6 @@
     <t>Visa Payment</t>
   </si>
   <si>
-    <t>02/28</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>8oz</t>
+  </si>
+  <si>
+    <t>04/28</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:AL14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
@@ -775,19 +775,19 @@
         <v>45</v>
       </c>
       <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
         <v>68</v>
-      </c>
-      <c r="M2" t="s">
-        <v>69</v>
       </c>
       <c r="N2" t="s">
         <v>51</v>
       </c>
       <c r="O2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="Q2">
         <v>9999999999</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -840,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -848,7 +848,7 @@
         <v>46</v>
       </c>
       <c r="U5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>47</v>
@@ -857,41 +857,41 @@
         <v>1</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:38">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="U6" t="s">
         <v>40</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Y6" s="4"/>
     </row>
     <row r="7" spans="1:38">
       <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="U7" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="V7" s="5">
         <v>1</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="20.25">
       <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="U8" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="U8" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="V8" s="5" t="s">
         <v>47</v>
@@ -900,10 +900,10 @@
     </row>
     <row r="9" spans="1:38">
       <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="U9" t="s">
         <v>58</v>
-      </c>
-      <c r="U9" t="s">
-        <v>59</v>
       </c>
       <c r="V9" s="5" t="s">
         <v>47</v>
@@ -912,13 +912,13 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U10" t="s">
+        <v>58</v>
+      </c>
+      <c r="V10" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="U10" t="s">
-        <v>59</v>
-      </c>
-      <c r="V10" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="Y10" s="4"/>
     </row>
@@ -936,19 +936,19 @@
         <v>41</v>
       </c>
       <c r="L11" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" t="s">
         <v>68</v>
-      </c>
-      <c r="M11" t="s">
-        <v>69</v>
       </c>
       <c r="N11" t="s">
         <v>51</v>
       </c>
       <c r="O11" t="s">
+        <v>69</v>
+      </c>
+      <c r="P11" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="Q11">
         <v>9898989898</v>
@@ -962,15 +962,15 @@
         <v>47</v>
       </c>
       <c r="S12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="T12" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:38">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>42</v>
@@ -981,28 +981,28 @@
     </row>
     <row r="14" spans="1:38">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
         <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L14" t="s">
+        <v>67</v>
+      </c>
+      <c r="M14" t="s">
         <v>68</v>
-      </c>
-      <c r="M14" t="s">
-        <v>69</v>
       </c>
       <c r="N14" t="s">
         <v>51</v>
       </c>
       <c r="O14" t="s">
+        <v>69</v>
+      </c>
+      <c r="P14" s="5" t="s">
         <v>70</v>
-      </c>
-      <c r="P14" s="5" t="s">
-        <v>71</v>
       </c>
       <c r="Q14">
         <v>9999999999</v>

</xml_diff>

<commit_message>
9 testcase for curlsmith
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1370A751-8062-4B22-A03D-B28DADC40F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFB7687-ADDA-45ED-BAD7-A2BB88665A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
   <si>
     <t>UserName</t>
   </si>
@@ -223,18 +223,9 @@
     <t>No Tax Address</t>
   </si>
   <si>
-    <t>844 North Court</t>
-  </si>
-  <si>
-    <t>Albany</t>
-  </si>
-  <si>
     <t>New York</t>
   </si>
   <si>
-    <t>12211</t>
-  </si>
-  <si>
     <t>Configurable Product_2</t>
   </si>
   <si>
@@ -251,6 +242,30 @@
   </si>
   <si>
     <t>04/28</t>
+  </si>
+  <si>
+    <t>1200 Waters Place</t>
+  </si>
+  <si>
+    <t>Bronx</t>
+  </si>
+  <si>
+    <t>10461</t>
+  </si>
+  <si>
+    <t>Configurable Product_2qty</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Simple_product_2qty</t>
+  </si>
+  <si>
+    <t>Bundle_Product_2qty</t>
+  </si>
+  <si>
+    <t>Mini 2 fl oz.</t>
   </si>
 </sst>
 </file>
@@ -605,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL14"/>
+  <dimension ref="A1:AL17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
@@ -775,19 +790,19 @@
         <v>45</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="N2" t="s">
         <v>51</v>
       </c>
       <c r="O2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="Q2">
         <v>9999999999</v>
@@ -840,7 +855,7 @@
         <v>1</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:38">
@@ -848,7 +863,7 @@
         <v>46</v>
       </c>
       <c r="U5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>47</v>
@@ -857,53 +872,53 @@
         <v>1</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:38">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="U6" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Y6" s="4"/>
     </row>
     <row r="7" spans="1:38">
       <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="U7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" t="s">
+        <v>40</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y7" s="4"/>
+    </row>
+    <row r="8" spans="1:38">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="V8" s="5">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="V7" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:38" ht="20.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="9" spans="1:38" ht="20.25">
+      <c r="A9" t="s">
         <v>61</v>
       </c>
-      <c r="U8" s="7" t="s">
+      <c r="U9" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="V8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y8" s="4"/>
-    </row>
-    <row r="9" spans="1:38">
-      <c r="A9" t="s">
-        <v>57</v>
-      </c>
-      <c r="U9" t="s">
-        <v>58</v>
       </c>
       <c r="V9" s="5" t="s">
         <v>47</v>
@@ -912,99 +927,135 @@
     </row>
     <row r="10" spans="1:38">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="U10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="Y10" s="4"/>
     </row>
     <row r="11" spans="1:38">
       <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" t="s">
-        <v>67</v>
-      </c>
-      <c r="M11" t="s">
-        <v>68</v>
-      </c>
-      <c r="N11" t="s">
-        <v>51</v>
-      </c>
-      <c r="O11" t="s">
-        <v>69</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q11">
-        <v>9898989898</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="U11" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y11" s="4"/>
     </row>
     <row r="12" spans="1:38">
       <c r="A12" t="s">
-        <v>54</v>
-      </c>
-      <c r="R12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="U12" t="s">
+        <v>58</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="1:38">
       <c r="A13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="U13" t="s">
+        <v>58</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y13" s="4"/>
     </row>
     <row r="14" spans="1:38">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
-        <v>60</v>
+      <c r="K14" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="L14" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="M14" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="N14" t="s">
         <v>51</v>
       </c>
       <c r="O14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="Q14">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N17" t="s">
+        <v>51</v>
+      </c>
+      <c r="O17" t="s">
+        <v>67</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q17">
         <v>9999999999</v>
       </c>
     </row>
@@ -1014,9 +1065,9 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6EC0626A-93FF-4B75-9E55-AED6062E6D4B}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{F0A4EEF5-EEBE-4FF0-BB4D-64D8943AC215}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
-    <hyperlink ref="K11" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
-    <hyperlink ref="B13" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
-    <hyperlink ref="D13" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
+    <hyperlink ref="K14" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
+    <hyperlink ref="B16" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
+    <hyperlink ref="D16" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
13 testcase for curlsmith
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFB7687-ADDA-45ED-BAD7-A2BB88665A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D25350-07B9-439A-9FE7-230F3D2717D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
   <si>
     <t>UserName</t>
   </si>
@@ -266,6 +266,15 @@
   </si>
   <si>
     <t>Mini 2 fl oz.</t>
+  </si>
+  <si>
+    <t>Child_Bundle</t>
+  </si>
+  <si>
+    <t>Double Cream Deep Quencher</t>
+  </si>
+  <si>
+    <t>Configurable_Bundle_child</t>
   </si>
 </sst>
 </file>
@@ -620,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL17"/>
+  <dimension ref="A1:AL19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
@@ -939,123 +948,145 @@
     </row>
     <row r="11" spans="1:38">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="U11" t="s">
-        <v>58</v>
-      </c>
-      <c r="V11" s="5" t="s">
-        <v>47</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="V11" s="5"/>
       <c r="Y11" s="4"/>
     </row>
     <row r="12" spans="1:38">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="U12" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="1:38">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="U13" t="s">
         <v>58</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="Y13" s="4"/>
     </row>
     <row r="14" spans="1:38">
       <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L14" t="s">
-        <v>74</v>
-      </c>
-      <c r="M14" t="s">
-        <v>75</v>
-      </c>
-      <c r="N14" t="s">
-        <v>51</v>
-      </c>
-      <c r="O14" t="s">
-        <v>67</v>
-      </c>
-      <c r="P14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q14">
-        <v>9898989898</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="U14" t="s">
+        <v>58</v>
+      </c>
+      <c r="V14" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y14" s="4"/>
     </row>
     <row r="15" spans="1:38">
       <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="R15" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="T15" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="U15" t="s">
+        <v>58</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y15" s="4"/>
     </row>
     <row r="16" spans="1:38">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L16" t="s">
+        <v>74</v>
+      </c>
+      <c r="M16" t="s">
+        <v>75</v>
+      </c>
+      <c r="N16" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" t="s">
+        <v>67</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q16">
+        <v>9898989898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
-      <c r="A17" t="s">
+    <row r="19" spans="1:20">
+      <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F19" t="s">
         <v>44</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G19" t="s">
         <v>60</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L19" t="s">
         <v>74</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M19" t="s">
         <v>75</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N19" t="s">
         <v>51</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O19" t="s">
         <v>67</v>
       </c>
-      <c r="P17" s="5" t="s">
+      <c r="P19" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="Q17">
+      <c r="Q19">
         <v>9999999999</v>
       </c>
     </row>
@@ -1065,9 +1096,9 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6EC0626A-93FF-4B75-9E55-AED6062E6D4B}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{F0A4EEF5-EEBE-4FF0-BB4D-64D8943AC215}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
-    <hyperlink ref="K14" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
-    <hyperlink ref="B16" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
-    <hyperlink ref="D16" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
+    <hyperlink ref="K16" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
+    <hyperlink ref="B18" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
+    <hyperlink ref="D18" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
6th testcase changes for the curlsmith
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D25350-07B9-439A-9FE7-230F3D2717D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA38AF50-5491-4881-9DFE-B62CDD50D21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6510" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
   <si>
     <t>UserName</t>
   </si>
@@ -142,9 +142,6 @@
     <t>AccountDetails</t>
   </si>
   <si>
-    <t>Curl Defining Styling Soufflé (Mini 2 fl oz.)</t>
-  </si>
-  <si>
     <t>vnarra@helenoftroy.com</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>Simple_Product</t>
   </si>
   <si>
-    <t>Hair Makeup - Turquoise</t>
-  </si>
-  <si>
     <t>Different_Bill_Ship</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t>Hold Me Softly Style Balm</t>
   </si>
   <si>
-    <t>Curl Defining Styling Soufflé</t>
-  </si>
-  <si>
     <t>Full 8 fl oz.</t>
   </si>
   <si>
@@ -275,6 +266,12 @@
   </si>
   <si>
     <t>Configurable_Bundle_child</t>
+  </si>
+  <si>
+    <t>Simple_product_1qty</t>
+  </si>
+  <si>
+    <t>vegan-silk-scarf</t>
   </si>
 </sst>
 </file>
@@ -629,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL19"/>
+  <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
@@ -781,37 +778,37 @@
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
-        <v>45</v>
-      </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q2">
         <v>9999999999</v>
@@ -819,32 +816,32 @@
     </row>
     <row r="3" spans="1:38">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="s">
-        <v>45</v>
-      </c>
       <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" t="s">
         <v>49</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>50</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>51</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="Q3">
         <v>9898989898</v>
@@ -855,238 +852,248 @@
         <v>38</v>
       </c>
       <c r="U4" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X4">
         <v>1</v>
       </c>
       <c r="Y4" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:38">
       <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" t="s">
+        <v>67</v>
+      </c>
+      <c r="V5" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="U5" t="s">
-        <v>70</v>
-      </c>
-      <c r="V5" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="X5">
         <v>1</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:38">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="U6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="V6" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Y6" s="4"/>
     </row>
     <row r="7" spans="1:38">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="U7" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="Y7" s="4"/>
     </row>
     <row r="8" spans="1:38">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="V8" s="5">
         <v>1</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="20.25">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U9" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y9" s="4"/>
     </row>
     <row r="10" spans="1:38">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="U10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="V10" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="Y10" s="4"/>
     </row>
     <row r="11" spans="1:38">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="U11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="V11" s="5"/>
       <c r="Y11" s="4"/>
     </row>
     <row r="12" spans="1:38">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="U12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y12" s="4"/>
     </row>
     <row r="13" spans="1:38">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="U13" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="V13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y13" s="4"/>
     </row>
     <row r="14" spans="1:38">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="U14" t="s">
-        <v>58</v>
-      </c>
-      <c r="V14" s="5" t="s">
-        <v>78</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="V14" s="5"/>
       <c r="Y14" s="4"/>
     </row>
     <row r="15" spans="1:38">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="U15" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="V15" s="5" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="Y15" s="4"/>
     </row>
     <row r="16" spans="1:38">
       <c r="A16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" t="s">
-        <v>44</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L16" t="s">
-        <v>74</v>
-      </c>
-      <c r="M16" t="s">
-        <v>75</v>
-      </c>
-      <c r="N16" t="s">
-        <v>51</v>
-      </c>
-      <c r="O16" t="s">
-        <v>67</v>
-      </c>
-      <c r="P16" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q16">
-        <v>9898989898</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="U16" t="s">
+        <v>83</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y16" s="4"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>54</v>
-      </c>
-      <c r="R17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="S17" s="6" t="s">
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L17" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" t="s">
+        <v>72</v>
+      </c>
+      <c r="N17" t="s">
+        <v>50</v>
+      </c>
+      <c r="O17" t="s">
+        <v>65</v>
+      </c>
+      <c r="P17" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="T17" s="5" t="s">
-        <v>55</v>
+      <c r="Q17">
+        <v>9898989898</v>
       </c>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>53</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="S18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" t="s">
-        <v>60</v>
-      </c>
-      <c r="L19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M19" t="s">
-        <v>75</v>
-      </c>
-      <c r="N19" t="s">
-        <v>51</v>
-      </c>
-      <c r="O19" t="s">
-        <v>67</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q19">
+        <v>55</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" t="s">
+        <v>71</v>
+      </c>
+      <c r="M20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N20" t="s">
+        <v>50</v>
+      </c>
+      <c r="O20" t="s">
+        <v>65</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q20">
         <v>9999999999</v>
       </c>
     </row>
@@ -1096,9 +1103,9 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6EC0626A-93FF-4B75-9E55-AED6062E6D4B}"/>
     <hyperlink ref="C2" r:id="rId3" xr:uid="{F0A4EEF5-EEBE-4FF0-BB4D-64D8943AC215}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
-    <hyperlink ref="K16" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
-    <hyperlink ref="B18" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
-    <hyperlink ref="D18" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
+    <hyperlink ref="K17" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
+    <hyperlink ref="B19" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
+    <hyperlink ref="D19" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
2 testcase related to the curlsmith
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA38AF50-5491-4881-9DFE-B62CDD50D21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593A4918-16C1-480C-8F85-0F4A6CD4FA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="2025" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
   <si>
     <t>UserName</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>vegan-silk-scarf</t>
+  </si>
+  <si>
+    <t>abogi@helenoftroy.com</t>
+  </si>
+  <si>
+    <t>Abcd@123</t>
   </si>
 </sst>
 </file>
@@ -629,7 +635,7 @@
   <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
@@ -778,16 +784,16 @@
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
         <v>43</v>
@@ -1101,13 +1107,12 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{CC7365F0-057F-4E26-AB1D-C83143B00E3B}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{6EC0626A-93FF-4B75-9E55-AED6062E6D4B}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{F0A4EEF5-EEBE-4FF0-BB4D-64D8943AC215}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
-    <hyperlink ref="K17" r:id="rId5" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
-    <hyperlink ref="B19" r:id="rId6" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
-    <hyperlink ref="D19" r:id="rId7" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{48F6E7BD-1564-4182-A09C-904682D5FD56}"/>
+    <hyperlink ref="K17" r:id="rId4" xr:uid="{C6354AE0-3B2A-41DD-BCE5-E5980F229A5B}"/>
+    <hyperlink ref="B19" r:id="rId5" xr:uid="{FE99142B-011B-4234-912A-686A7B9CD164}"/>
+    <hyperlink ref="D19" r:id="rId6" xr:uid="{48AD6B6A-66C2-4956-BF9D-F7635F0B0308}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Curlsmith E2E changes excel product changes
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
+++ b/src/test/resources/TestData/Curlsmith/CurlsmithTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593A4918-16C1-480C-8F85-0F4A6CD4FA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE5EBB5-A4E9-451E-8CE9-FF71120C5F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="87">
   <si>
     <t>UserName</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Abcd@123</t>
+  </si>
+  <si>
+    <t>super-slip-pre-biotic-primer</t>
   </si>
 </sst>
 </file>
@@ -635,12 +638,12 @@
   <dimension ref="A1:AL20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -875,7 +878,7 @@
         <v>45</v>
       </c>
       <c r="U5" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="V5" s="5" t="s">
         <v>46</v>
@@ -976,7 +979,7 @@
         <v>56</v>
       </c>
       <c r="U13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="V13" s="5" t="s">
         <v>46</v>

</xml_diff>